<commit_message>
portfolio page with avg. cost, total cost
</commit_message>
<xml_diff>
--- a/Profit_Intel/wwwroot/Upload/sampledata.xlsx
+++ b/Profit_Intel/wwwroot/Upload/sampledata.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28810"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eddy\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muhammadsaadan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{344E5FF3-58A2-40CE-A424-73228C98A223}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10005" yWindow="2880" windowWidth="14595" windowHeight="18330" xr2:uid="{42C5781E-D1FD-4573-A79E-6D703563EC38}"/>
+    <workbookView xWindow="10000" yWindow="460" windowWidth="14600" windowHeight="14620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -68,7 +73,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -434,23 +439,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C6769D-9901-4EE3-AAF3-FC6F2035E19F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -467,7 +472,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43491</v>
       </c>
@@ -484,7 +489,7 @@
         <v>71.55</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43492</v>
       </c>
@@ -501,7 +506,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43493</v>
       </c>
@@ -518,7 +523,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43494</v>
       </c>
@@ -526,16 +531,16 @@
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2">
-        <v>2.1852</v>
+        <v>33.5321</v>
       </c>
       <c r="E5" s="3">
         <v>65.900000000000006</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43495</v>
       </c>
@@ -552,7 +557,7 @@
         <v>91.08</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43496</v>
       </c>
@@ -569,7 +574,7 @@
         <v>90.9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43497</v>
       </c>
@@ -586,7 +591,7 @@
         <v>91.13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43498</v>
       </c>
@@ -603,7 +608,7 @@
         <v>89.65</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43499</v>
       </c>
@@ -620,7 +625,7 @@
         <v>89.32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43500</v>
       </c>
@@ -637,7 +642,7 @@
         <v>89.55</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43501</v>
       </c>
@@ -654,7 +659,7 @@
         <v>89.44</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43502</v>
       </c>
@@ -671,7 +676,7 @@
         <v>94.75</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43503</v>
       </c>
@@ -688,7 +693,7 @@
         <v>94.59</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43504</v>
       </c>
@@ -705,7 +710,7 @@
         <v>99.53</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43505</v>
       </c>
@@ -722,7 +727,7 @@
         <v>88.03</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43506</v>
       </c>
@@ -739,7 +744,7 @@
         <v>101.43</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43507</v>
       </c>
@@ -750,13 +755,13 @@
         <v>9</v>
       </c>
       <c r="D18" s="2">
-        <v>1.8239000000000001</v>
+        <v>8.2939000000000007</v>
       </c>
       <c r="E18" s="3">
         <v>101.43</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43508</v>
       </c>
@@ -773,7 +778,7 @@
         <v>117.85</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43509</v>
       </c>
@@ -790,7 +795,7 @@
         <v>113.5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43510</v>
       </c>
@@ -807,7 +812,7 @@
         <v>113.31</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43511</v>
       </c>
@@ -824,7 +829,7 @@
         <v>103.63</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43512</v>
       </c>
@@ -841,7 +846,7 @@
         <v>103.61</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43513</v>
       </c>
@@ -858,7 +863,7 @@
         <v>103.2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>43514</v>
       </c>
@@ -875,7 +880,7 @@
         <v>101.42</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>43515</v>
       </c>
@@ -892,7 +897,7 @@
         <v>87.72</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43516</v>
       </c>
@@ -909,7 +914,7 @@
         <v>91.5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>43517</v>
       </c>
@@ -920,13 +925,13 @@
         <v>9</v>
       </c>
       <c r="D28" s="2">
-        <v>0.7</v>
+        <v>3.7</v>
       </c>
       <c r="E28" s="3">
         <v>91.36</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>43518</v>
       </c>
@@ -943,7 +948,7 @@
         <v>86.75</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>43519</v>
       </c>
@@ -960,7 +965,7 @@
         <v>87.91</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>43520</v>
       </c>
@@ -977,7 +982,7 @@
         <v>76.680000000000007</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>43521</v>
       </c>
@@ -994,7 +999,7 @@
         <v>77.77</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>43522</v>
       </c>
@@ -1011,7 +1016,7 @@
         <v>77.930000000000007</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>43523</v>
       </c>
@@ -1028,7 +1033,7 @@
         <v>73.349999999999994</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>43524</v>
       </c>
@@ -1045,7 +1050,7 @@
         <v>52.41</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>43525</v>
       </c>
@@ -1062,7 +1067,7 @@
         <v>52.34</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>43526</v>
       </c>
@@ -1079,7 +1084,7 @@
         <v>44.85</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>43527</v>
       </c>
@@ -1096,7 +1101,7 @@
         <v>52.21</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>43528</v>
       </c>
@@ -1113,7 +1118,7 @@
         <v>48.38</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>43529</v>
       </c>
@@ -1130,7 +1135,7 @@
         <v>49.49</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>43530</v>
       </c>

</xml_diff>

<commit_message>
Removed taxes page, updated Ratio handling, capital gains tax is now funcitonal and can be found on portfolio page
</commit_message>
<xml_diff>
--- a/Profit_Intel/wwwroot/Upload/sampledata.xlsx
+++ b/Profit_Intel/wwwroot/Upload/sampledata.xlsx
@@ -1,28 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28810"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muhammadsaadan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eddy\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{344E5FF3-58A2-40CE-A424-73228C98A223}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10000" yWindow="460" windowWidth="14600" windowHeight="14620"/>
+    <workbookView xWindow="10005" yWindow="2880" windowWidth="14595" windowHeight="18330" xr2:uid="{42C5781E-D1FD-4573-A79E-6D703563EC38}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -73,7 +68,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -439,23 +434,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C6769D-9901-4EE3-AAF3-FC6F2035E19F}">
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,7 +467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43491</v>
       </c>
@@ -489,7 +484,7 @@
         <v>71.55</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43492</v>
       </c>
@@ -506,7 +501,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43493</v>
       </c>
@@ -523,7 +518,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43494</v>
       </c>
@@ -531,16 +526,16 @@
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2">
-        <v>33.5321</v>
+        <v>2.1852</v>
       </c>
       <c r="E5" s="3">
         <v>65.900000000000006</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43495</v>
       </c>
@@ -557,7 +552,7 @@
         <v>91.08</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43496</v>
       </c>
@@ -574,7 +569,7 @@
         <v>90.9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43497</v>
       </c>
@@ -591,7 +586,7 @@
         <v>91.13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43498</v>
       </c>
@@ -608,7 +603,7 @@
         <v>89.65</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43499</v>
       </c>
@@ -625,7 +620,7 @@
         <v>89.32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43500</v>
       </c>
@@ -642,7 +637,7 @@
         <v>89.55</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43501</v>
       </c>
@@ -659,7 +654,7 @@
         <v>89.44</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43502</v>
       </c>
@@ -676,7 +671,7 @@
         <v>94.75</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43503</v>
       </c>
@@ -693,7 +688,7 @@
         <v>94.59</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43504</v>
       </c>
@@ -710,7 +705,7 @@
         <v>99.53</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43505</v>
       </c>
@@ -727,7 +722,7 @@
         <v>88.03</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43506</v>
       </c>
@@ -744,7 +739,7 @@
         <v>101.43</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43507</v>
       </c>
@@ -755,13 +750,13 @@
         <v>9</v>
       </c>
       <c r="D18" s="2">
-        <v>8.2939000000000007</v>
+        <v>1.8239000000000001</v>
       </c>
       <c r="E18" s="3">
         <v>101.43</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43508</v>
       </c>
@@ -778,7 +773,7 @@
         <v>117.85</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43509</v>
       </c>
@@ -795,7 +790,7 @@
         <v>113.5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43510</v>
       </c>
@@ -812,7 +807,7 @@
         <v>113.31</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43511</v>
       </c>
@@ -829,7 +824,7 @@
         <v>103.63</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43512</v>
       </c>
@@ -846,7 +841,7 @@
         <v>103.61</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43513</v>
       </c>
@@ -863,7 +858,7 @@
         <v>103.2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43514</v>
       </c>
@@ -880,7 +875,7 @@
         <v>101.42</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43515</v>
       </c>
@@ -897,7 +892,7 @@
         <v>87.72</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43516</v>
       </c>
@@ -914,7 +909,7 @@
         <v>91.5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43517</v>
       </c>
@@ -925,13 +920,13 @@
         <v>9</v>
       </c>
       <c r="D28" s="2">
-        <v>3.7</v>
+        <v>0.7</v>
       </c>
       <c r="E28" s="3">
         <v>91.36</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43518</v>
       </c>
@@ -948,7 +943,7 @@
         <v>86.75</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43519</v>
       </c>
@@ -965,7 +960,7 @@
         <v>87.91</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43520</v>
       </c>
@@ -982,7 +977,7 @@
         <v>76.680000000000007</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43521</v>
       </c>
@@ -999,7 +994,7 @@
         <v>77.77</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43522</v>
       </c>
@@ -1016,7 +1011,7 @@
         <v>77.930000000000007</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43523</v>
       </c>
@@ -1033,7 +1028,7 @@
         <v>73.349999999999994</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43524</v>
       </c>
@@ -1050,7 +1045,7 @@
         <v>52.41</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43525</v>
       </c>
@@ -1067,7 +1062,7 @@
         <v>52.34</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43526</v>
       </c>
@@ -1084,7 +1079,7 @@
         <v>44.85</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43527</v>
       </c>
@@ -1101,7 +1096,7 @@
         <v>52.21</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43528</v>
       </c>
@@ -1118,7 +1113,7 @@
         <v>48.38</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43529</v>
       </c>
@@ -1135,7 +1130,7 @@
         <v>49.49</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43530</v>
       </c>

</xml_diff>

<commit_message>
Update date from portfolio (needs work)
</commit_message>
<xml_diff>
--- a/Profit_Intel/wwwroot/Upload/sampledata.xlsx
+++ b/Profit_Intel/wwwroot/Upload/sampledata.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28810"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eddy\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muhammadsaadan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{344E5FF3-58A2-40CE-A424-73228C98A223}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10005" yWindow="2880" windowWidth="14595" windowHeight="18330" xr2:uid="{42C5781E-D1FD-4573-A79E-6D703563EC38}"/>
+    <workbookView xWindow="10000" yWindow="460" windowWidth="14600" windowHeight="14620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -68,7 +73,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -434,23 +439,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C6769D-9901-4EE3-AAF3-FC6F2035E19F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -467,7 +472,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43491</v>
       </c>
@@ -484,7 +489,7 @@
         <v>71.55</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43492</v>
       </c>
@@ -501,7 +506,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43493</v>
       </c>
@@ -518,7 +523,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43494</v>
       </c>
@@ -526,16 +531,16 @@
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2">
-        <v>2.1852</v>
+        <v>33.5321</v>
       </c>
       <c r="E5" s="3">
         <v>65.900000000000006</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43495</v>
       </c>
@@ -552,7 +557,7 @@
         <v>91.08</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43496</v>
       </c>
@@ -569,7 +574,7 @@
         <v>90.9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43497</v>
       </c>
@@ -586,7 +591,7 @@
         <v>91.13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43498</v>
       </c>
@@ -603,7 +608,7 @@
         <v>89.65</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43499</v>
       </c>
@@ -620,7 +625,7 @@
         <v>89.32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43500</v>
       </c>
@@ -637,7 +642,7 @@
         <v>89.55</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43501</v>
       </c>
@@ -654,7 +659,7 @@
         <v>89.44</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43502</v>
       </c>
@@ -671,7 +676,7 @@
         <v>94.75</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43503</v>
       </c>
@@ -688,7 +693,7 @@
         <v>94.59</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43504</v>
       </c>
@@ -705,7 +710,7 @@
         <v>99.53</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43505</v>
       </c>
@@ -722,7 +727,7 @@
         <v>88.03</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43506</v>
       </c>
@@ -739,7 +744,7 @@
         <v>101.43</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43507</v>
       </c>
@@ -750,13 +755,13 @@
         <v>9</v>
       </c>
       <c r="D18" s="2">
-        <v>1.8239000000000001</v>
+        <v>8.2939000000000007</v>
       </c>
       <c r="E18" s="3">
         <v>101.43</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43508</v>
       </c>
@@ -773,7 +778,7 @@
         <v>117.85</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43509</v>
       </c>
@@ -790,7 +795,7 @@
         <v>113.5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43510</v>
       </c>
@@ -807,7 +812,7 @@
         <v>113.31</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43511</v>
       </c>
@@ -824,7 +829,7 @@
         <v>103.63</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43512</v>
       </c>
@@ -841,7 +846,7 @@
         <v>103.61</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43513</v>
       </c>
@@ -858,7 +863,7 @@
         <v>103.2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>43514</v>
       </c>
@@ -875,7 +880,7 @@
         <v>101.42</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>43515</v>
       </c>
@@ -892,7 +897,7 @@
         <v>87.72</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43516</v>
       </c>
@@ -909,7 +914,7 @@
         <v>91.5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>43517</v>
       </c>
@@ -920,13 +925,13 @@
         <v>9</v>
       </c>
       <c r="D28" s="2">
-        <v>0.7</v>
+        <v>3.7</v>
       </c>
       <c r="E28" s="3">
         <v>91.36</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>43518</v>
       </c>
@@ -943,7 +948,7 @@
         <v>86.75</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>43519</v>
       </c>
@@ -960,7 +965,7 @@
         <v>87.91</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>43520</v>
       </c>
@@ -977,7 +982,7 @@
         <v>76.680000000000007</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>43521</v>
       </c>
@@ -994,7 +999,7 @@
         <v>77.77</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>43522</v>
       </c>
@@ -1011,7 +1016,7 @@
         <v>77.930000000000007</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>43523</v>
       </c>
@@ -1028,7 +1033,7 @@
         <v>73.349999999999994</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>43524</v>
       </c>
@@ -1045,7 +1050,7 @@
         <v>52.41</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>43525</v>
       </c>
@@ -1062,7 +1067,7 @@
         <v>52.34</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>43526</v>
       </c>
@@ -1079,7 +1084,7 @@
         <v>44.85</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>43527</v>
       </c>
@@ -1096,7 +1101,7 @@
         <v>52.21</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>43528</v>
       </c>
@@ -1113,7 +1118,7 @@
         <v>48.38</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>43529</v>
       </c>
@@ -1130,7 +1135,7 @@
         <v>49.49</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>43530</v>
       </c>

</xml_diff>